<commit_message>
subindo versão final site
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPTECH\Projeto Individual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPTECH\Projeto Individual\Projeto Individual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED08DD6C-0BE2-4D28-AD61-EEE285459CCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5B0C5A-6FFE-4955-8BDF-7A93335826EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7C8D7172-7E11-47EF-95DB-85B8CFE4CDE5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
   <si>
     <t>Requisito</t>
   </si>
@@ -110,9 +110,6 @@
     <t>Fazer protótipo da Dashboard</t>
   </si>
   <si>
-    <t>Fazer Dashboard em página HTML</t>
-  </si>
-  <si>
     <t>Essencial</t>
   </si>
   <si>
@@ -147,6 +144,21 @@
   </si>
   <si>
     <t>Criar as cartas dos personagens de anime que farão parte dos pacotes na interação do site</t>
+  </si>
+  <si>
+    <t>Fazer diagrama técnico</t>
+  </si>
+  <si>
+    <t>Fazer o diagrama de solução técnico com as etapas do serviço realizado</t>
+  </si>
+  <si>
+    <t>Configurar i banco de dados MySQL para rodar na VM virtual box</t>
+  </si>
+  <si>
+    <t>Fazer o sistema de interação do site com o usuário</t>
+  </si>
+  <si>
+    <t>Criar as rotas, fazendo as conexões do front end com o banco de dados</t>
   </si>
 </sst>
 </file>
@@ -224,7 +236,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -247,11 +259,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -271,6 +294,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -674,7 +701,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -731,9 +758,9 @@
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
@@ -747,9 +774,9 @@
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="4"/>
       <c r="C4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -763,9 +790,9 @@
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -779,14 +806,14 @@
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="4" t="s">
-        <v>10</v>
+      <c r="F6" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="4"/>
@@ -795,14 +822,14 @@
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="4" t="s">
-        <v>10</v>
+      <c r="F7" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="4">
@@ -813,14 +840,14 @@
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="4"/>
       <c r="C8" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="4" t="s">
-        <v>10</v>
+      <c r="F8" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="4">
@@ -831,14 +858,14 @@
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="4"/>
       <c r="C9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="4" t="s">
-        <v>10</v>
+      <c r="F9" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="4">
@@ -849,16 +876,16 @@
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="5" t="s">
-        <v>28</v>
+      <c r="F10" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="4">
@@ -869,16 +896,16 @@
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>33</v>
+      <c r="B11" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="5" t="s">
-        <v>28</v>
+      <c r="F11" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="4">
@@ -889,9 +916,9 @@
       <c r="A12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" s="4"/>
       <c r="C12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -907,14 +934,16 @@
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="2"/>
+      <c r="B13" s="4" t="s">
+        <v>40</v>
+      </c>
       <c r="C13" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="5" t="s">
-        <v>28</v>
+      <c r="F13" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="4">
@@ -925,14 +954,14 @@
       <c r="A14" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="4"/>
       <c r="C14" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="5" t="s">
-        <v>28</v>
+      <c r="F14" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="4">
@@ -941,16 +970,18 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>28</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="C15" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="5" t="s">
-        <v>28</v>
+      <c r="F15" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="4">
@@ -961,14 +992,16 @@
       <c r="A16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="4" t="s">
+        <v>38</v>
+      </c>
       <c r="C16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="4" t="s">
-        <v>10</v>
+      <c r="F16" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="4">
@@ -979,61 +1012,63 @@
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="C17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="5" t="s">
-        <v>28</v>
+      <c r="F17" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G17" s="2"/>
-      <c r="H17" s="4">
-        <v>1</v>
-      </c>
+      <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>32</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="B18" s="4"/>
       <c r="C18" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="5" t="s">
-        <v>28</v>
+      <c r="F18" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B19" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="B19" s="4"/>
       <c r="C19" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="4" t="s">
-        <v>10</v>
+      <c r="F19" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="G19" s="2"/>
-      <c r="H19" s="4"/>
+      <c r="H19" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="C20" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1041,27 +1076,21 @@
         <v>9</v>
       </c>
       <c r="G20" s="2"/>
-      <c r="H20" s="4">
-        <v>1</v>
-      </c>
+      <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="8" t="s">
         <v>36</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>37</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G21" s="2"/>
-      <c r="H21" s="4"/>
+      <c r="F21" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>